<commit_message>
Upload do projeto e dados para Banca
</commit_message>
<xml_diff>
--- a/Arquivos e resultados/5 - Analise/Analise_Manual_SQL_excel_2023-05-28 15-02-34.xlsx
+++ b/Arquivos e resultados/5 - Analise/Analise_Manual_SQL_excel_2023-05-28 15-02-34.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\TCC\TCC II - Everson Leonardi\Projeto\Dados\Analise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\TCC\TCC II - Everson Leonardi\Projeto\ACI40\Arquivos e resultados\5 - Analise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEF2EE3-1AD6-4572-9644-11A2C6AAF025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8C9F48-F989-4760-B056-CC4D91316FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="352">
   <si>
     <t>id</t>
   </si>
@@ -1172,6 +1172,9 @@
   </si>
   <si>
     <t>[['IoT connectivity solutions', 103, 129, 'Target']]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1223,11 +1226,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1236,6 +1248,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1538,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1568,7 @@
     <col min="6" max="6" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1572,8 +1587,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -1596,7 +1614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>99</v>
       </c>
@@ -1619,7 +1637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>98</v>
       </c>
@@ -1642,7 +1660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>97</v>
       </c>
@@ -1665,7 +1683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>96</v>
       </c>
@@ -1688,7 +1706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>95</v>
       </c>
@@ -1711,7 +1729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>94</v>
       </c>
@@ -1734,7 +1752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>93</v>
       </c>
@@ -1757,7 +1775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>92</v>
       </c>
@@ -1780,7 +1798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>91</v>
       </c>
@@ -1803,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>90</v>
       </c>
@@ -1826,7 +1844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>89</v>
       </c>
@@ -1849,7 +1867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>88</v>
       </c>
@@ -1872,7 +1890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>87</v>
       </c>
@@ -1895,7 +1913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>86</v>
       </c>

</xml_diff>